<commit_message>
add log and update error code
</commit_message>
<xml_diff>
--- a/proj04_touringdemo/data/MY19R_Social_footer_link.xlsx
+++ b/proj04_touringdemo/data/MY19R_Social_footer_link.xlsx
@@ -752,13 +752,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="35.81640625" customWidth="1"/>
+    <col min="1" max="4" width="35.81640625" customWidth="1"/>
+    <col min="5" max="5" width="70.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>